<commit_message>
update illustrative DC for Banks image
</commit_message>
<xml_diff>
--- a/MODS-DC-Generators/Illustrative-MODS-Generator-NEW/Illustrative_Images_DC17.xlsx
+++ b/MODS-DC-Generators/Illustrative-MODS-Generator-NEW/Illustrative_Images_DC17.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24760" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="24660" windowHeight="15360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8564" uniqueCount="2255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8571" uniqueCount="2259">
   <si>
     <t>liv_013001</t>
   </si>
@@ -6784,6 +6784,18 @@
   </si>
   <si>
     <t>Adrian S. Wisnicki, Justin Livingstone, and Heather F. Ball at University of Glasgow Library, 2017</t>
+  </si>
+  <si>
+    <t>liv_016252</t>
+  </si>
+  <si>
+    <t>Nigel Banks, 2017</t>
+  </si>
+  <si>
+    <t>Banks, Nigel</t>
+  </si>
+  <si>
+    <t>Copyright Nigel Banks. Creative Commons Attribution-NonCommercial 3.0 Unported (https://creativecommons.org/licenses/by-nc/3.0/).</t>
   </si>
 </sst>
 </file>
@@ -6796,6 +6808,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -6900,7 +6913,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="416">
+  <cellStyleXfs count="422">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -6962,6 +6975,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -7387,7 +7406,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="416">
+  <cellStyles count="422">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -7604,6 +7623,9 @@
     <cellStyle name="Followed Hyperlink" xfId="411" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="413" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="415" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="417" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="419" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="421" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -7803,6 +7825,9 @@
     <cellStyle name="Hyperlink" xfId="410" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="412" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="414" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="416" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="418" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="420" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -8132,11 +8157,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1189"/>
+  <dimension ref="A1:I1190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1177" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1168" sqref="I1168:I1188"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1183" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1190" sqref="A1190:I1190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -40303,6 +40328,32 @@
         <v>1920</v>
       </c>
     </row>
+    <row r="1190" spans="1:9" ht="30">
+      <c r="A1190" s="22" t="s">
+        <v>2255</v>
+      </c>
+      <c r="B1190" s="10" t="s">
+        <v>2256</v>
+      </c>
+      <c r="C1190" s="7" t="s">
+        <v>2257</v>
+      </c>
+      <c r="D1190" s="6" t="s">
+        <v>669</v>
+      </c>
+      <c r="E1190" s="7" t="s">
+        <v>664</v>
+      </c>
+      <c r="F1190" s="8">
+        <v>2017</v>
+      </c>
+      <c r="G1190" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="I1190" s="21" t="s">
+        <v>2258</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:I802">
     <sortCondition ref="A2:A802"/>

</xml_diff>

<commit_message>
Add slave stick Illus DC
</commit_message>
<xml_diff>
--- a/MODS-DC-Generators/Illustrative-MODS-Generator-NEW/Illustrative_Images_DC17.xlsx
+++ b/MODS-DC-Generators/Illustrative-MODS-Generator-NEW/Illustrative_Images_DC17.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24900" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="24640" windowHeight="15360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8634" uniqueCount="2282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8641" uniqueCount="2285">
   <si>
     <t>liv_013001</t>
   </si>
@@ -6865,6 +6865,15 @@
   </si>
   <si>
     <t>Copyright Lewis Walter. Used by permission.</t>
+  </si>
+  <si>
+    <t>liv_016262</t>
+  </si>
+  <si>
+    <t>Slave stick, reportedly removed by David Livingstone from the neck of a slave, 1840-1870</t>
+  </si>
+  <si>
+    <t>Copyright David Livingstone Centre. May not be reproduced without the express written consent of the National Trust for Scotland, on behalf of the Scottish National Memorial to David Livingstone Trust.</t>
   </si>
 </sst>
 </file>
@@ -6981,7 +6990,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="446">
+  <cellStyleXfs count="448">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -7428,8 +7437,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -7503,8 +7514,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="446">
+  <cellStyles count="448">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -7736,6 +7750,7 @@
     <cellStyle name="Followed Hyperlink" xfId="441" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="443" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="445" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="447" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -7950,6 +7965,7 @@
     <cellStyle name="Hyperlink" xfId="440" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="442" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="444" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="446" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -8279,11 +8295,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1199"/>
+  <dimension ref="A1:I1200"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1186" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1199" sqref="I1199"/>
+      <pane ySplit="1" topLeftCell="A1195" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1200" sqref="I1200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -40710,6 +40726,32 @@
         <v>2281</v>
       </c>
     </row>
+    <row r="1200" spans="1:9" ht="45">
+      <c r="A1200" s="22" t="s">
+        <v>2282</v>
+      </c>
+      <c r="B1200" s="23" t="s">
+        <v>2283</v>
+      </c>
+      <c r="C1200" s="13" t="s">
+        <v>682</v>
+      </c>
+      <c r="D1200" s="6" t="s">
+        <v>669</v>
+      </c>
+      <c r="E1200" s="7" t="s">
+        <v>664</v>
+      </c>
+      <c r="F1200" s="8">
+        <v>1840</v>
+      </c>
+      <c r="G1200" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="I1200" s="25" t="s">
+        <v>2284</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:I802">
     <sortCondition ref="A2:A802"/>

</xml_diff>

<commit_message>
update Illustrative DC excel
</commit_message>
<xml_diff>
--- a/MODS-DC-Generators/Illustrative-MODS-Generator-NEW/Illustrative_Images_DC17.xlsx
+++ b/MODS-DC-Generators/Illustrative-MODS-Generator-NEW/Illustrative_Images_DC17.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="24640" windowHeight="15360" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24900" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8641" uniqueCount="2285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8690" uniqueCount="2295">
   <si>
     <t>liv_013001</t>
   </si>
@@ -6874,6 +6874,36 @@
   </si>
   <si>
     <t>Copyright David Livingstone Centre. May not be reproduced without the express written consent of the National Trust for Scotland, on behalf of the Scottish National Memorial to David Livingstone Trust.</t>
+  </si>
+  <si>
+    <t>liv_016263</t>
+  </si>
+  <si>
+    <t>liv_016264</t>
+  </si>
+  <si>
+    <t>liv_016265</t>
+  </si>
+  <si>
+    <t>liv_016266</t>
+  </si>
+  <si>
+    <t>liv_016267</t>
+  </si>
+  <si>
+    <t>liv_016268</t>
+  </si>
+  <si>
+    <t>liv_016269</t>
+  </si>
+  <si>
+    <t>Auction advertisement for David Livingstone, Letter to Richard Owen, 26 December 1864, [1970s?]</t>
+  </si>
+  <si>
+    <t>Elmer L. Andersen Library, University of Minnesota, 2018</t>
+  </si>
+  <si>
+    <t>Archival box that holds Livingstone manuscript, Elmer L. Andersen Library, University of Minnesota, 2018</t>
   </si>
 </sst>
 </file>
@@ -6990,7 +7020,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="448">
+  <cellStyleXfs count="472">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -7052,6 +7082,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -7518,7 +7572,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="448">
+  <cellStyles count="472">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -7751,6 +7805,18 @@
     <cellStyle name="Followed Hyperlink" xfId="443" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="445" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="447" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="449" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="451" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="453" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="455" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="457" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="459" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="461" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="463" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="465" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="467" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="469" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="471" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -7966,6 +8032,18 @@
     <cellStyle name="Hyperlink" xfId="442" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="444" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="446" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="448" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="450" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="452" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="454" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="456" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="458" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="460" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="462" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="464" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="466" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="468" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="470" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -8295,11 +8373,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1200"/>
+  <dimension ref="A1:I1207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1195" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1200" sqref="I1200"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1196" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1212" sqref="B1212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -40752,6 +40830,188 @@
         <v>2284</v>
       </c>
     </row>
+    <row r="1201" spans="1:9" ht="30">
+      <c r="A1201" s="22" t="s">
+        <v>2285</v>
+      </c>
+      <c r="B1201" s="10" t="s">
+        <v>2293</v>
+      </c>
+      <c r="C1201" s="7" t="s">
+        <v>1740</v>
+      </c>
+      <c r="D1201" s="6" t="s">
+        <v>669</v>
+      </c>
+      <c r="E1201" s="7" t="s">
+        <v>664</v>
+      </c>
+      <c r="F1201" s="8">
+        <v>2018</v>
+      </c>
+      <c r="G1201" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="I1201" s="21" t="s">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="1202" spans="1:9" ht="30">
+      <c r="A1202" s="22" t="s">
+        <v>2286</v>
+      </c>
+      <c r="B1202" s="10" t="s">
+        <v>2293</v>
+      </c>
+      <c r="C1202" s="7" t="s">
+        <v>1740</v>
+      </c>
+      <c r="D1202" s="6" t="s">
+        <v>669</v>
+      </c>
+      <c r="E1202" s="7" t="s">
+        <v>664</v>
+      </c>
+      <c r="F1202" s="8">
+        <v>2018</v>
+      </c>
+      <c r="G1202" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="I1202" s="21" t="s">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:9" ht="30">
+      <c r="A1203" s="22" t="s">
+        <v>2287</v>
+      </c>
+      <c r="B1203" s="10" t="s">
+        <v>2293</v>
+      </c>
+      <c r="C1203" s="7" t="s">
+        <v>1740</v>
+      </c>
+      <c r="D1203" s="6" t="s">
+        <v>669</v>
+      </c>
+      <c r="E1203" s="7" t="s">
+        <v>664</v>
+      </c>
+      <c r="F1203" s="8">
+        <v>2018</v>
+      </c>
+      <c r="G1203" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="I1203" s="21" t="s">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:9" ht="30">
+      <c r="A1204" s="22" t="s">
+        <v>2288</v>
+      </c>
+      <c r="B1204" s="10" t="s">
+        <v>2293</v>
+      </c>
+      <c r="C1204" s="7" t="s">
+        <v>1740</v>
+      </c>
+      <c r="D1204" s="6" t="s">
+        <v>669</v>
+      </c>
+      <c r="E1204" s="7" t="s">
+        <v>664</v>
+      </c>
+      <c r="F1204" s="8">
+        <v>2018</v>
+      </c>
+      <c r="G1204" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="I1204" s="21" t="s">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:9" ht="30">
+      <c r="A1205" s="22" t="s">
+        <v>2289</v>
+      </c>
+      <c r="B1205" s="10" t="s">
+        <v>2293</v>
+      </c>
+      <c r="C1205" s="7" t="s">
+        <v>1740</v>
+      </c>
+      <c r="D1205" s="6" t="s">
+        <v>669</v>
+      </c>
+      <c r="E1205" s="7" t="s">
+        <v>664</v>
+      </c>
+      <c r="F1205" s="8">
+        <v>2018</v>
+      </c>
+      <c r="G1205" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="I1205" s="21" t="s">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:9" ht="30">
+      <c r="A1206" s="22" t="s">
+        <v>2290</v>
+      </c>
+      <c r="B1206" s="10" t="s">
+        <v>2294</v>
+      </c>
+      <c r="C1206" s="7" t="s">
+        <v>1740</v>
+      </c>
+      <c r="D1206" s="6" t="s">
+        <v>669</v>
+      </c>
+      <c r="E1206" s="7" t="s">
+        <v>664</v>
+      </c>
+      <c r="F1206" s="8">
+        <v>2018</v>
+      </c>
+      <c r="G1206" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="I1206" s="21" t="s">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="1207" spans="1:9" ht="30">
+      <c r="A1207" s="22" t="s">
+        <v>2291</v>
+      </c>
+      <c r="B1207" s="10" t="s">
+        <v>2292</v>
+      </c>
+      <c r="C1207" s="7" t="s">
+        <v>1740</v>
+      </c>
+      <c r="D1207" s="6" t="s">
+        <v>669</v>
+      </c>
+      <c r="E1207" s="7" t="s">
+        <v>664</v>
+      </c>
+      <c r="F1207" s="8">
+        <v>2018</v>
+      </c>
+      <c r="G1207" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="I1207" s="21" t="s">
+        <v>1929</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:I802">
     <sortCondition ref="A2:A802"/>

</xml_diff>